<commit_message>
issue: error and stretch calc and plot
</commit_message>
<xml_diff>
--- a/excel/64grid_diameter14test.xlsx
+++ b/excel/64grid_diameter14test.xlsx
@@ -471,7 +471,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -505,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.3571428571428572</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4107142857142858</v>
+        <v>0.3214285714285715</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -556,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3749999999999999</v>
+        <v>0.4285714285714286</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -573,7 +573,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3214285714285714</v>
+        <v>0.3839285714285715</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
@@ -590,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3839285714285714</v>
+        <v>0.2857142857142858</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.3169642857142858</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3928571428571428</v>
+        <v>0.3660714285714286</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
@@ -641,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3214285714285715</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0.03571428571428571</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5535714285714286</v>
+        <v>0.3035714285714286</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -692,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5</v>
+        <v>0.4464285714285715</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2678571428571428</v>
+        <v>0.25</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3839285714285714</v>
+        <v>0.375</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -743,7 +743,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3705357142857143</v>
+        <v>0.3526785714285714</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3125000000000001</v>
+        <v>0.3705357142857143</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.359375</v>
+        <v>0.3236607142857143</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3750000000000001</v>
+        <v>0.3861607142857144</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6071428571428571</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -828,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4642857142857143</v>
+        <v>0.3928571428571428</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3035714285714286</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="E24" t="n">
         <v>1</v>
@@ -862,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2678571428571428</v>
+        <v>0.125</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0.2321428571428572</v>
+        <v>0.4732142857142857</v>
       </c>
       <c r="E26" t="n">
         <v>1</v>
@@ -896,7 +896,7 @@
         <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>0.375</v>
+        <v>0.3214285714285715</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -913,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>0.3660714285714285</v>
+        <v>0.3080357142857142</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
@@ -930,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>0.3705357142857142</v>
+        <v>0.3616071428571428</v>
       </c>
       <c r="E29" t="n">
         <v>1</v>
@@ -947,7 +947,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0.3750000000000001</v>
+        <v>0.3571428571428571</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -964,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>0.3482142857142856</v>
+        <v>0.3705357142857142</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0.03571428571428571</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="E32" t="n">
         <v>1</v>
@@ -998,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2142857142857143</v>
+        <v>0.3214285714285714</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0.3749999999999999</v>
+        <v>0.3035714285714285</v>
       </c>
       <c r="E34" t="n">
         <v>1</v>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="n">
-        <v>0.2321428571428572</v>
+        <v>0.4285714285714286</v>
       </c>
       <c r="E35" t="n">
         <v>1</v>
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0.2678571428571428</v>
+        <v>0.25</v>
       </c>
       <c r="E36" t="n">
         <v>1</v>
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>0.2678571428571428</v>
+        <v>0.2767857142857142</v>
       </c>
       <c r="E37" t="n">
         <v>1</v>
@@ -1083,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3616071428571428</v>
+        <v>0.4017857142857144</v>
       </c>
       <c r="E38" t="n">
         <v>1</v>
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>0.3392857142857143</v>
+        <v>0.2589285714285714</v>
       </c>
       <c r="E39" t="n">
         <v>1</v>
@@ -1117,7 +1117,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>0.3281249999999999</v>
+        <v>0.3459821428571428</v>
       </c>
       <c r="E40" t="n">
         <v>1</v>
@@ -1134,7 +1134,7 @@
         <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>0.3415178571428571</v>
+        <v>0.3727678571428571</v>
       </c>
       <c r="E41" t="n">
         <v>1</v>
@@ -1151,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>0.75</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="E42" t="n">
         <v>1</v>
@@ -1168,7 +1168,7 @@
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="E43" t="n">
         <v>1</v>
@@ -1185,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>0.2321428571428572</v>
+        <v>0.3035714285714286</v>
       </c>
       <c r="E44" t="n">
         <v>1</v>
@@ -1202,7 +1202,7 @@
         <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>0.2142857142857143</v>
+        <v>0.2678571428571428</v>
       </c>
       <c r="E45" t="n">
         <v>1</v>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>0.4464285714285714</v>
+        <v>0.3303571428571428</v>
       </c>
       <c r="E46" t="n">
         <v>1</v>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0.3392857142857142</v>
+        <v>0.5178571428571428</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
@@ -1253,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.3303571428571429</v>
+        <v>0.4062499999999999</v>
       </c>
       <c r="E48" t="n">
         <v>1</v>
@@ -1270,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>0.3883928571428572</v>
+        <v>0.4464285714285714</v>
       </c>
       <c r="E49" t="n">
         <v>1</v>
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>0.3750000000000001</v>
+        <v>0.2946428571428572</v>
       </c>
       <c r="E50" t="n">
         <v>1</v>
@@ -1304,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="D51" t="n">
-        <v>0.3169642857142857</v>
+        <v>0.3593749999999999</v>
       </c>
       <c r="E51" t="n">
         <v>1</v>
@@ -1321,7 +1321,7 @@
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>0.3928571428571428</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="E52" t="n">
         <v>1</v>
@@ -1338,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1071428571428571</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="E53" t="n">
         <v>1</v>
@@ -1355,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2678571428571428</v>
+        <v>0.3392857142857143</v>
       </c>
       <c r="E54" t="n">
         <v>1</v>
@@ -1372,7 +1372,7 @@
         <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>0.3392857142857143</v>
+        <v>0.3571428571428572</v>
       </c>
       <c r="E55" t="n">
         <v>1</v>
@@ -1389,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>0.2678571428571428</v>
+        <v>0.3571428571428572</v>
       </c>
       <c r="E56" t="n">
         <v>1</v>
@@ -1406,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>0.2946428571428571</v>
+        <v>0.3392857142857142</v>
       </c>
       <c r="E57" t="n">
         <v>1</v>
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>0.3705357142857142</v>
+        <v>0.3794642857142856</v>
       </c>
       <c r="E58" t="n">
         <v>1</v>
@@ -1440,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="D59" t="n">
-        <v>0.3616071428571428</v>
+        <v>0.3883928571428572</v>
       </c>
       <c r="E59" t="n">
         <v>1</v>
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0.408482142857143</v>
+        <v>0.3526785714285714</v>
       </c>
       <c r="E60" t="n">
         <v>1</v>
@@ -1474,7 +1474,7 @@
         <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>0.3995535714285713</v>
+        <v>0.3973214285714285</v>
       </c>
       <c r="E61" t="n">
         <v>1</v>

</xml_diff>